<commit_message>
update the tables in the report
</commit_message>
<xml_diff>
--- a/pcsk9/doc/raw_dir_condi_meta.xlsx
+++ b/pcsk9/doc/raw_dir_condi_meta.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="270">
   <si>
     <t>SNP</t>
   </si>
@@ -780,6 +780,60 @@
   <si>
     <t>RSID</t>
   </si>
+  <si>
+    <t>STUDY</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>meta_0</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>+++-+  ++</t>
+  </si>
+  <si>
+    <t>meta_1</t>
+  </si>
+  <si>
+    <t>meta_2</t>
+  </si>
+  <si>
+    <t>meta_3</t>
+  </si>
+  <si>
+    <t>rint_0</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>rint_1</t>
+  </si>
+  <si>
+    <t>rint_2</t>
+  </si>
+  <si>
+    <t>rint_3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>---+-  --</t>
+  </si>
 </sst>
 </file>
 
@@ -29187,13 +29241,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -30354,6 +30421,690 @@
       </c>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>252</v>
+      </c>
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>253</v>
+      </c>
+      <c r="G41" t="s">
+        <v>254</v>
+      </c>
+      <c r="H41" t="s">
+        <v>227</v>
+      </c>
+      <c r="I41" t="s">
+        <v>224</v>
+      </c>
+      <c r="J41" t="s">
+        <v>225</v>
+      </c>
+      <c r="K41" t="s">
+        <v>226</v>
+      </c>
+      <c r="L41" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>55496039</v>
+      </c>
+      <c r="E42">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>256</v>
+      </c>
+      <c r="G42" t="s">
+        <v>257</v>
+      </c>
+      <c r="H42" t="s">
+        <v>258</v>
+      </c>
+      <c r="I42">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="J42">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="K42">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="L42">
+        <v>2.1489999999999999E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>55496039</v>
+      </c>
+      <c r="E43">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>256</v>
+      </c>
+      <c r="G43" t="s">
+        <v>257</v>
+      </c>
+      <c r="H43" t="s">
+        <v>258</v>
+      </c>
+      <c r="I43">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J43">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="K43">
+        <v>3.8059999999999997E-2</v>
+      </c>
+      <c r="L43">
+        <v>6.8939999999999995E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>260</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>55496039</v>
+      </c>
+      <c r="E44">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>256</v>
+      </c>
+      <c r="G44" t="s">
+        <v>257</v>
+      </c>
+      <c r="H44" t="s">
+        <v>258</v>
+      </c>
+      <c r="I44">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="J44">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="K44">
+        <v>3.2579999999999998E-2</v>
+      </c>
+      <c r="L44">
+        <v>3.251E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>55496039</v>
+      </c>
+      <c r="E45">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>256</v>
+      </c>
+      <c r="G45" t="s">
+        <v>257</v>
+      </c>
+      <c r="H45" t="s">
+        <v>258</v>
+      </c>
+      <c r="I45">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="J45">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K45">
+        <v>2.9690000000000001E-2</v>
+      </c>
+      <c r="L45">
+        <v>7.9310000000000005E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>55496039</v>
+      </c>
+      <c r="E46">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>256</v>
+      </c>
+      <c r="G46" t="s">
+        <v>257</v>
+      </c>
+      <c r="H46" t="s">
+        <v>263</v>
+      </c>
+      <c r="I46">
+        <v>6.3880000000000006E-2</v>
+      </c>
+      <c r="J46">
+        <v>2.052E-2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>263</v>
+      </c>
+      <c r="L46">
+        <v>1.854E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>55496039</v>
+      </c>
+      <c r="E47">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>256</v>
+      </c>
+      <c r="G47" t="s">
+        <v>257</v>
+      </c>
+      <c r="H47" t="s">
+        <v>263</v>
+      </c>
+      <c r="I47">
+        <v>7.0660000000000001E-2</v>
+      </c>
+      <c r="J47">
+        <v>2.043E-2</v>
+      </c>
+      <c r="K47" t="s">
+        <v>263</v>
+      </c>
+      <c r="L47">
+        <v>5.4259999999999996E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>55496039</v>
+      </c>
+      <c r="E48">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>256</v>
+      </c>
+      <c r="G48" t="s">
+        <v>257</v>
+      </c>
+      <c r="H48" t="s">
+        <v>263</v>
+      </c>
+      <c r="I48">
+        <v>3.6839999999999998E-2</v>
+      </c>
+      <c r="J48">
+        <v>2.138E-2</v>
+      </c>
+      <c r="K48" t="s">
+        <v>263</v>
+      </c>
+      <c r="L48">
+        <v>8.4879999999999997E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>266</v>
+      </c>
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>55496039</v>
+      </c>
+      <c r="E49">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>256</v>
+      </c>
+      <c r="G49" t="s">
+        <v>257</v>
+      </c>
+      <c r="H49" t="s">
+        <v>263</v>
+      </c>
+      <c r="I49">
+        <v>3.9210000000000002E-2</v>
+      </c>
+      <c r="J49">
+        <v>2.145E-2</v>
+      </c>
+      <c r="K49" t="s">
+        <v>263</v>
+      </c>
+      <c r="L49">
+        <v>6.7530000000000007E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>252</v>
+      </c>
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>253</v>
+      </c>
+      <c r="G51" t="s">
+        <v>254</v>
+      </c>
+      <c r="H51" t="s">
+        <v>227</v>
+      </c>
+      <c r="I51" t="s">
+        <v>224</v>
+      </c>
+      <c r="J51" t="s">
+        <v>225</v>
+      </c>
+      <c r="K51" t="s">
+        <v>226</v>
+      </c>
+      <c r="L51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>55504650</v>
+      </c>
+      <c r="E52">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F52" t="s">
+        <v>267</v>
+      </c>
+      <c r="G52" t="s">
+        <v>268</v>
+      </c>
+      <c r="H52" t="s">
+        <v>269</v>
+      </c>
+      <c r="I52">
+        <v>-6.4000000000000003E-3</v>
+      </c>
+      <c r="J52">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K52">
+        <v>0.73650000000000004</v>
+      </c>
+      <c r="L52">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>55504650</v>
+      </c>
+      <c r="E53">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F53" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" t="s">
+        <v>268</v>
+      </c>
+      <c r="H53" t="s">
+        <v>269</v>
+      </c>
+      <c r="I53">
+        <v>-1.4800000000000001E-2</v>
+      </c>
+      <c r="J53">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K53">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="L53">
+        <v>3.2649999999999998E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>260</v>
+      </c>
+      <c r="B54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>55504650</v>
+      </c>
+      <c r="E54">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F54" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" t="s">
+        <v>268</v>
+      </c>
+      <c r="H54" t="s">
+        <v>269</v>
+      </c>
+      <c r="I54">
+        <v>-1.1900000000000001E-2</v>
+      </c>
+      <c r="J54">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K54">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="L54">
+        <v>8.9020000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>261</v>
+      </c>
+      <c r="B55" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>55504650</v>
+      </c>
+      <c r="E55">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F55" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" t="s">
+        <v>268</v>
+      </c>
+      <c r="H55" t="s">
+        <v>269</v>
+      </c>
+      <c r="I55">
+        <v>-1.4200000000000001E-2</v>
+      </c>
+      <c r="J55">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K55">
+        <v>0.85119999999999996</v>
+      </c>
+      <c r="L55">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>55504650</v>
+      </c>
+      <c r="E56">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F56" t="s">
+        <v>267</v>
+      </c>
+      <c r="G56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H56" t="s">
+        <v>263</v>
+      </c>
+      <c r="I56">
+        <v>-9.3740000000000004E-3</v>
+      </c>
+      <c r="J56">
+        <v>1.023E-2</v>
+      </c>
+      <c r="K56" t="s">
+        <v>263</v>
+      </c>
+      <c r="L56">
+        <v>0.35959999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>264</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>55504650</v>
+      </c>
+      <c r="E57">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F57" t="s">
+        <v>267</v>
+      </c>
+      <c r="G57" t="s">
+        <v>268</v>
+      </c>
+      <c r="H57" t="s">
+        <v>263</v>
+      </c>
+      <c r="I57">
+        <v>-2.2429999999999999E-2</v>
+      </c>
+      <c r="J57">
+        <v>1.022E-2</v>
+      </c>
+      <c r="K57" t="s">
+        <v>263</v>
+      </c>
+      <c r="L57">
+        <v>2.8170000000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>265</v>
+      </c>
+      <c r="B58" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>55504650</v>
+      </c>
+      <c r="E58">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F58" t="s">
+        <v>267</v>
+      </c>
+      <c r="G58" t="s">
+        <v>268</v>
+      </c>
+      <c r="H58" t="s">
+        <v>263</v>
+      </c>
+      <c r="I58">
+        <v>-7.9559999999999995E-3</v>
+      </c>
+      <c r="J58">
+        <v>1.0529999999999999E-2</v>
+      </c>
+      <c r="K58" t="s">
+        <v>263</v>
+      </c>
+      <c r="L58">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>266</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>55504650</v>
+      </c>
+      <c r="E59">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F59" t="s">
+        <v>267</v>
+      </c>
+      <c r="G59" t="s">
+        <v>268</v>
+      </c>
+      <c r="H59" t="s">
+        <v>263</v>
+      </c>
+      <c r="I59">
+        <v>-9.9690000000000004E-3</v>
+      </c>
+      <c r="J59">
+        <v>1.057E-2</v>
+      </c>
+      <c r="K59" t="s">
+        <v>263</v>
+      </c>
+      <c r="L59">
+        <v>0.34560000000000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>